<commit_message>
Dokumentation stand 18.12.2023 (seitenregelung)
</commit_message>
<xml_diff>
--- a/Dokumentation/Kopie von Auto_ESY.xlsx
+++ b/Dokumentation/Kopie von Auto_ESY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Gruppe_05\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFBB805-E61F-4805-9167-E561E5635811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A591CED-E16B-46F6-BC1F-F88CA868A74B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="241">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1147,6 +1147,18 @@
   </si>
   <si>
     <t>Mit den Code nach Fehlern und Ideen geholfen - Selber nicht geschrieben, nur Tipps gegeben</t>
+  </si>
+  <si>
+    <t>Den code Weiterergänzt (versucht ein eigenes algoritmus zu erstellen --&gt; nicht funktionsfäh.) Nach erfolglosen versuch neues konzept angefangen (seitenregelung) funktioniert halbgwegs (macht unnötige kreise) hat aber die gesamt Strecke geschafft</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie beim Jovic versucht einen Algorithmus selbst zu erstellen -&gt; Fehlerhaft. </t>
+  </si>
+  <si>
+    <t>Fehlersuche beim eigenen Code -&gt; Ergebnisse: Werte zu hoch/niedrig? Unterprogramme falsch? Fehler wurde noch nicht gefunden</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1551,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1854,12 +1866,42 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1869,36 +1911,6 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1922,6 +1934,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2408,14 +2423,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="119" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2464,10 +2479,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="109"/>
+      <c r="F7" s="114"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2478,8 +2493,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2488,8 +2503,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2498,8 +2513,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2508,8 +2523,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="113"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2530,49 +2545,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="115"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="115"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="115"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115"/>
-      <c r="F18" s="115"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="120"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2585,64 +2600,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="121"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109" t="s">
+      <c r="B26" s="114"/>
+      <c r="C26" s="114"/>
+      <c r="D26" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="114"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117" t="s">
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="109" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="118"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="110"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2653,16 +2678,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2722,7 +2737,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2736,11 +2751,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="123" t="s">
@@ -2970,7 +2985,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="138" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,7 +3077,9 @@
       <c r="B10" s="40">
         <v>45271</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="40">
+        <v>45278</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3561,8 +3578,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="63" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3576,16 +3593,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="119" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4028,12 +4045,16 @@
       <c r="D23" s="103">
         <v>1</v>
       </c>
-      <c r="E23" s="62"/>
+      <c r="E23" s="62">
+        <v>0.5</v>
+      </c>
       <c r="F23" s="62"/>
       <c r="G23" s="39">
         <v>45264</v>
       </c>
-      <c r="H23" s="62"/>
+      <c r="H23" s="131">
+        <v>45271</v>
+      </c>
       <c r="I23" s="63"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4049,12 +4070,16 @@
       <c r="D24" s="103">
         <v>0.75</v>
       </c>
-      <c r="E24" s="62"/>
+      <c r="E24" s="62" t="s">
+        <v>238</v>
+      </c>
       <c r="F24" s="62"/>
       <c r="G24" s="39">
         <v>45264</v>
       </c>
-      <c r="H24" s="62"/>
+      <c r="H24" s="131" t="s">
+        <v>238</v>
+      </c>
       <c r="I24" s="63"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -4070,12 +4095,16 @@
       <c r="D25" s="103">
         <v>0.5</v>
       </c>
-      <c r="E25" s="62"/>
+      <c r="E25" s="62" t="s">
+        <v>238</v>
+      </c>
       <c r="F25" s="62"/>
       <c r="G25" s="39">
         <v>45264</v>
       </c>
-      <c r="H25" s="62"/>
+      <c r="H25" s="131" t="s">
+        <v>238</v>
+      </c>
       <c r="I25" s="63"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -4091,12 +4120,16 @@
       <c r="D26" s="103">
         <v>0.25</v>
       </c>
-      <c r="E26" s="62"/>
+      <c r="E26" s="62">
+        <v>0.15</v>
+      </c>
       <c r="F26" s="62"/>
       <c r="G26" s="39">
         <v>45264</v>
       </c>
-      <c r="H26" s="62"/>
+      <c r="H26" s="131">
+        <v>45271</v>
+      </c>
       <c r="I26" s="63"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4112,12 +4145,16 @@
       <c r="D27" s="103">
         <v>3</v>
       </c>
-      <c r="E27" s="62"/>
+      <c r="E27" s="62">
+        <v>3</v>
+      </c>
       <c r="F27" s="62"/>
       <c r="G27" s="40">
         <v>45271</v>
       </c>
-      <c r="H27" s="62"/>
+      <c r="H27" s="131">
+        <v>45278</v>
+      </c>
       <c r="I27" s="63"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4138,7 +4175,7 @@
       <c r="G28" s="39">
         <v>45278</v>
       </c>
-      <c r="H28" s="62"/>
+      <c r="H28" s="131"/>
       <c r="I28" s="63">
         <v>0</v>
       </c>
@@ -4236,7 +4273,7 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>5</v>
+        <v>8.65</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
@@ -5849,7 +5886,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6148,20 +6185,40 @@
       <c r="C16" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="2"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="2"/>
+      <c r="E16" s="40">
+        <v>45278</v>
+      </c>
+      <c r="F16" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B17" s="41">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E17" s="40">
+        <v>45278</v>
+      </c>
+      <c r="F17" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="40">
+        <v>45271</v>
+      </c>
       <c r="B18" s="41"/>
       <c r="C18" s="2"/>
       <c r="E18" s="41"/>
@@ -6169,7 +6226,9 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="40">
+        <v>45271</v>
+      </c>
       <c r="B19" s="41"/>
       <c r="C19" s="2"/>
       <c r="E19" s="41"/>
@@ -6177,7 +6236,9 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="40">
+        <v>45271</v>
+      </c>
       <c r="B20" s="41"/>
       <c r="C20" s="2"/>
       <c r="E20" s="41"/>

</xml_diff>

<commit_message>
Dokumentation von 08.01.2024 Ohne den gesamten teil von Valenzuela
</commit_message>
<xml_diff>
--- a/Dokumentation/Kopie von Auto_ESY.xlsx
+++ b/Dokumentation/Kopie von Auto_ESY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Gruppe_05\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\001150\Documents\group-05\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A591CED-E16B-46F6-BC1F-F88CA868A74B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB65078-67EB-44E9-9207-C0DA50F4598F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="244">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1159,6 +1159,15 @@
   </si>
   <si>
     <t>Fehlersuche beim eigenen Code -&gt; Ergebnisse: Werte zu hoch/niedrig? Unterprogramme falsch? Fehler wurde noch nicht gefunden</t>
+  </si>
+  <si>
+    <t>Die Sensoren liefern Stabile werte</t>
+  </si>
+  <si>
+    <t>Technische Probleme beim Anmelden (neuer Profil + das verknüpfen mit dem alten Z laufwerk) dazu musste noch Sourcetree nochmal heruntergeladen werden + verknüpfen etc.</t>
+  </si>
+  <si>
+    <t>Neues Konzept für das autonome fahren (idee: mit &amp;&amp; in der If schleife (right + left + Center IR) damit es fährt (konnte nicht getestet werden da die batterie leer ist</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1560,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1866,6 +1875,36 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1884,33 +1923,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1934,9 +1949,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2423,14 +2435,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2479,10 +2491,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="114" t="s">
+      <c r="E7" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="114"/>
+      <c r="F7" s="111"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2493,8 +2505,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2503,8 +2515,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="121"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2513,8 +2525,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2523,8 +2535,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2545,49 +2557,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="117"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2600,74 +2612,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="113" t="s">
+      <c r="A23" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="113"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="123"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="114" t="s">
+      <c r="A26" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="114"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114" t="s">
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="109" t="s">
+      <c r="A27" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109" t="s">
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="119" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="110" t="s">
+      <c r="A29" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="110"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2678,6 +2680,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2751,29 +2763,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="123"/>
+      <c r="C3" s="125"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="123"/>
+      <c r="C4" s="125"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="123"/>
+      <c r="C5" s="125"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2982,10 +2994,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="138" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,11 +3008,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3008,18 +3020,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="126" t="s">
+      <c r="A4" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -3088,65 +3100,71 @@
       <c r="B11" s="39">
         <v>45278</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="40">
+        <v>45278</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
+      <c r="A12" s="108" t="s">
+        <v>241</v>
       </c>
       <c r="B12" s="39">
         <v>45306</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="39">
-        <v>45320</v>
+        <v>45306</v>
       </c>
       <c r="C13" s="41"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="39">
+        <v>45320</v>
+      </c>
+      <c r="C14" s="41"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B15" s="39">
         <v>45341</v>
       </c>
-      <c r="C14" s="41"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B16" s="39">
         <v>45355</v>
       </c>
-      <c r="C15" s="41"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="41"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B17" s="39">
         <v>45362</v>
       </c>
-      <c r="C16" s="41"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="41"/>
       <c r="C17" s="41"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="41"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3156,12 +3174,12 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="41"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3171,12 +3189,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="41"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3255,9 +3273,14 @@
       <c r="C40" s="41"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3293,14 +3316,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3593,16 +3616,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4052,7 +4075,7 @@
       <c r="G23" s="39">
         <v>45264</v>
       </c>
-      <c r="H23" s="131">
+      <c r="H23" s="109">
         <v>45271</v>
       </c>
       <c r="I23" s="63"/>
@@ -4077,7 +4100,7 @@
       <c r="G24" s="39">
         <v>45264</v>
       </c>
-      <c r="H24" s="131" t="s">
+      <c r="H24" s="109" t="s">
         <v>238</v>
       </c>
       <c r="I24" s="63"/>
@@ -4102,7 +4125,7 @@
       <c r="G25" s="39">
         <v>45264</v>
       </c>
-      <c r="H25" s="131" t="s">
+      <c r="H25" s="109" t="s">
         <v>238</v>
       </c>
       <c r="I25" s="63"/>
@@ -4127,7 +4150,7 @@
       <c r="G26" s="39">
         <v>45264</v>
       </c>
-      <c r="H26" s="131">
+      <c r="H26" s="109">
         <v>45271</v>
       </c>
       <c r="I26" s="63"/>
@@ -4152,7 +4175,7 @@
       <c r="G27" s="40">
         <v>45271</v>
       </c>
-      <c r="H27" s="131">
+      <c r="H27" s="109">
         <v>45278</v>
       </c>
       <c r="I27" s="63"/>
@@ -4175,7 +4198,7 @@
       <c r="G28" s="39">
         <v>45278</v>
       </c>
-      <c r="H28" s="131"/>
+      <c r="H28" s="109"/>
       <c r="I28" s="63">
         <v>0</v>
       </c>
@@ -4323,19 +4346,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="129" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
@@ -4999,16 +5022,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="126" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -5784,71 +5807,71 @@
       <c r="A21" s="93" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="129" t="s">
+      <c r="B21" s="131" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="129"/>
-      <c r="D21" s="129"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="130" t="s">
+      <c r="B22" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="130" t="s">
+      <c r="B23" s="132" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="130"/>
-      <c r="D23" s="130"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="130" t="s">
+      <c r="B24" s="132" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="130"/>
-      <c r="D24" s="130"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="95"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="95"/>
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="95"/>
-      <c r="B27" s="128"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
+      <c r="B27" s="130"/>
+      <c r="C27" s="130"/>
+      <c r="D27" s="130"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="95"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="128"/>
-      <c r="D28" s="128"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="95"/>
-      <c r="B29" s="128"/>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128"/>
+      <c r="B29" s="130"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5885,8 +5908,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5900,16 +5923,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="126" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="E1" s="124" t="s">
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="E1" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="35"/>
@@ -6215,22 +6238,36 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
-        <v>45271</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="2"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45299</v>
+      </c>
+      <c r="B18" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E18" s="40">
+        <v>45299</v>
+      </c>
+      <c r="F18" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="G18" s="108" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
-        <v>45271</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="2"/>
+        <v>45299</v>
+      </c>
+      <c r="B19" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>243</v>
+      </c>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
       <c r="G19" s="2"/>

</xml_diff>

<commit_message>
Stand 22.01.2024 nur pinbelegung von sensoren hat sich geänder + doku
</commit_message>
<xml_diff>
--- a/Dokumentation/Kopie von Auto_ESY.xlsx
+++ b/Dokumentation/Kopie von Auto_ESY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\001150\Documents\group-05\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170506\Documents\group-05\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB65078-67EB-44E9-9207-C0DA50F4598F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D76E0B-0229-47E5-895A-A66439844C31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="246">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1168,6 +1168,12 @@
   </si>
   <si>
     <t>Neues Konzept für das autonome fahren (idee: mit &amp;&amp; in der If schleife (right + left + Center IR) damit es fährt (konnte nicht getestet werden da die batterie leer ist</t>
+  </si>
+  <si>
+    <t>Fehlersucher da der rechte IR sensor keine stabile Werte zurückliefert ( Fehlersucher mit Prof. Jahn) 1. Lösung wert öfters ablesen und daraus einen mittelwert bilden --&gt; ein neue fehler der Sensor funktioniert gar nicht obwohl mehrere Sensoren versucht wurden.</t>
+  </si>
+  <si>
+    <t>Wegen Präsi und Erklärung von Prof. Jahn nur 2 Stunden Zeit gehabt -&gt; An Kabelung geholfen (Klimpen). Fehlersuche mit Jovic &amp; Prof. Jahn und besprechung von Noten</t>
   </si>
 </sst>
 </file>
@@ -1881,12 +1887,42 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1895,36 +1931,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2435,14 +2441,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2491,10 +2497,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2505,8 +2511,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2515,8 +2521,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2525,8 +2531,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2535,8 +2541,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2557,49 +2563,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2612,64 +2618,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2680,16 +2696,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2763,11 +2769,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="125" t="s">
@@ -3616,16 +3622,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5908,8 +5914,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6268,24 +6274,44 @@
       <c r="C19" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="40">
+        <v>45306</v>
+      </c>
+      <c r="F19" s="41">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
-        <v>45271</v>
-      </c>
-      <c r="B20" s="41"/>
+        <v>45306</v>
+      </c>
+      <c r="B20" s="41">
+        <v>3</v>
+      </c>
       <c r="C20" s="2"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="2"/>
+      <c r="E20" s="40">
+        <v>45313</v>
+      </c>
+      <c r="F20" s="41">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="40">
+        <v>45313</v>
+      </c>
+      <c r="B21" s="41">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>244</v>
+      </c>
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
       <c r="G21" s="2"/>

</xml_diff>

<commit_message>
Stand 11.03.2024 Werte sind stabil ausßer FrontSensor
</commit_message>
<xml_diff>
--- a/Dokumentation/Kopie von Auto_ESY.xlsx
+++ b/Dokumentation/Kopie von Auto_ESY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170506\Documents\group-05\neu\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170506\Documents\group-05\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B83B05D-1D0E-4CDC-A4BA-0BDDB50666BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FE6F5C-E4B8-4051-9EA5-1F11684E7C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="254">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1183,6 +1183,21 @@
   </si>
   <si>
     <t>Mit den Valenzuela eine neue Idee zu kriegen, damit die Strecke nicht lange dauert.</t>
+  </si>
+  <si>
+    <t>11.03.2024</t>
+  </si>
+  <si>
+    <t>Neues Algorithmuskonzept enwickelt (mittelregelung ohne den Center value)</t>
+  </si>
+  <si>
+    <t>Sensoren Werte mit dem Professor durchgegangen und implementiert</t>
+  </si>
+  <si>
+    <t>Neuen Code hergestellt mit Sensor-Werten vom Professor - Fehlgeschlagen -&gt; Auto fährt nicht richtig</t>
+  </si>
+  <si>
+    <t>Die Werte stabil ausgeben indem man sie in cm umgewandelt hat (frontsensor nicht funktionsfähig)und somit neues konzept mit if anweisungen in cm</t>
   </si>
 </sst>
 </file>
@@ -1575,7 +1590,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1899,12 +1914,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1914,36 +1959,6 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1967,6 +1982,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2453,14 +2474,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="122" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2509,10 +2530,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="112"/>
+      <c r="F7" s="117"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2523,8 +2544,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="113"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2533,8 +2554,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2543,8 +2564,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2553,8 +2574,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2575,49 +2596,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="117"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="121"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2630,64 +2651,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="124" t="s">
+      <c r="A23" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="124"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="112" t="s">
+      <c r="A26" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="112"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112" t="s">
+      <c r="B26" s="117"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="120"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="119"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="120" t="s">
+      <c r="B28" s="111"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="112" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="120"/>
-      <c r="F28" s="120"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
-      <c r="D29" s="122"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="122"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2698,16 +2729,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2781,11 +2802,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="126" t="s">
@@ -3634,16 +3655,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="122" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5926,8 +5947,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6364,28 +6385,52 @@
       <c r="C23" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="2"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="2"/>
+      <c r="E23" s="134" t="s">
+        <v>249</v>
+      </c>
+      <c r="F23" s="41">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="134" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" s="41">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" s="134" t="s">
+        <v>249</v>
+      </c>
+      <c r="F24" s="41">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="134" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="134"/>
       <c r="B26" s="41"/>
       <c r="C26" s="2"/>
       <c r="E26" s="41"/>
@@ -6393,7 +6438,7 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
+      <c r="A27" s="134"/>
       <c r="B27" s="41"/>
       <c r="C27" s="2"/>
       <c r="E27" s="41"/>
@@ -6401,7 +6446,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="134"/>
       <c r="B28" s="41"/>
       <c r="C28" s="2"/>
       <c r="E28" s="41"/>
@@ -6409,7 +6454,7 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="134"/>
       <c r="B29" s="41"/>
       <c r="C29" s="2"/>
       <c r="E29" s="41"/>
@@ -6417,7 +6462,7 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="134"/>
       <c r="B30" s="41"/>
       <c r="C30" s="2"/>
       <c r="E30" s="41"/>
@@ -6425,7 +6470,7 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="134"/>
       <c r="B31" s="41"/>
       <c r="C31" s="2"/>
       <c r="E31" s="41"/>
@@ -6433,7 +6478,7 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="134"/>
       <c r="B32" s="41"/>
       <c r="C32" s="2"/>
       <c r="E32" s="41"/>
@@ -6441,7 +6486,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
+      <c r="A33" s="135"/>
       <c r="B33" s="42"/>
       <c r="C33" s="24"/>
       <c r="E33" s="42"/>

</xml_diff>